<commit_message>
Implemented IListener class and screenshot functionality
</commit_message>
<xml_diff>
--- a/src/main/java/com/Dashboard/TestData/LoginTestData.xlsx
+++ b/src/main/java/com/Dashboard/TestData/LoginTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaheen Akhtar\git\repository\Dashboard\src\main\java\com\Dashboard\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B35F67-B037-429F-8DEA-A43F76F4E6E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86B5AEE-FE76-42AB-BE9D-FD9445BEB05B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9B270448-1A92-4C34-AABB-F2D6A45C5F02}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" xr2:uid="{9B270448-1A92-4C34-AABB-F2D6A45C5F02}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -93,7 +93,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -103,12 +103,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -144,8 +138,8 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -464,7 +458,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added upload album script
</commit_message>
<xml_diff>
--- a/src/main/java/com/Dashboard/TestData/LoginTestData.xlsx
+++ b/src/main/java/com/Dashboard/TestData/LoginTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaheen Akhtar\git\repository\Dashboard\src\main\java\com\Dashboard\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07D77669-14DC-4069-822E-37855EDDF635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77F8CF5-F79F-4EE0-B2B1-08B32A910913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="705" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{9B270448-1A92-4C34-AABB-F2D6A45C5F02}"/>
+    <workbookView xWindow="3240" yWindow="1395" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{5957173E-284D-47B6-A290-4C6493186F86}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Email</t>
   </si>
@@ -50,17 +50,23 @@
     <t>test@123</t>
   </si>
   <si>
-    <t>Album_Name</t>
+    <t>Add_Album</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
   <si>
     <t>test</t>
+  </si>
+  <si>
+    <t>Fest2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,43 +83,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF242424"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -121,31 +106,14 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -460,64 +428,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F784E2C6-D5DE-48DA-8E3F-8BD93FFE66DF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12940D30-8AEB-4E2D-8C72-6A29927993D2}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{DD2CD233-EBEE-40B6-92C4-85465AC12666}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{F9DBCB62-10BC-4718-8615-359CCC5E8E98}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{617DE787-1E80-497B-B6D4-D8753B5702A8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B1F98A5-5227-4E35-8749-4878AC779751}">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{286819FC-4A75-49C2-98B3-CF110C957342}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added change password module
</commit_message>
<xml_diff>
--- a/src/main/java/com/Dashboard/TestData/LoginTestData.xlsx
+++ b/src/main/java/com/Dashboard/TestData/LoginTestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaheen Akhtar\git\repository\Dashboard\src\main\java\com\Dashboard\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77F8CF5-F79F-4EE0-B2B1-08B32A910913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB1D9C4-4DDC-4E6E-9DCC-E3F5CFBED5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="1395" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{5957173E-284D-47B6-A290-4C6493186F86}"/>
+    <workbookView xWindow="2520" yWindow="1590" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{5957173E-284D-47B6-A290-4C6493186F86}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="AddAlbum" sheetId="2" r:id="rId2"/>
+    <sheet name="ChangePassword" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
   <si>
     <t>Email</t>
   </si>
@@ -47,9 +48,6 @@
     <t>dashboard@aimbeyond.com</t>
   </si>
   <si>
-    <t>test@123</t>
-  </si>
-  <si>
     <t>Add_Album</t>
   </si>
   <si>
@@ -60,13 +58,28 @@
   </si>
   <si>
     <t>Fest2</t>
+  </si>
+  <si>
+    <t>New Password</t>
+  </si>
+  <si>
+    <t>Old Password</t>
+  </si>
+  <si>
+    <t>Confirm Password</t>
+  </si>
+  <si>
+    <t>test123</t>
+  </si>
+  <si>
+    <t>test1234</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -76,13 +89,6 @@
     </font>
     <font>
       <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
@@ -113,7 +119,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -432,7 +438,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,16 +459,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{F9DBCB62-10BC-4718-8615-359CCC5E8E98}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{617DE787-1E80-497B-B6D4-D8753B5702A8}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -470,7 +472,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{286819FC-4A75-49C2-98B3-CF110C957342}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -481,21 +483,64 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A31C90-BF1A-46C7-859A-74A941160E3F}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added static wait in test case
</commit_message>
<xml_diff>
--- a/src/main/java/com/Dashboard/TestData/LoginTestData.xlsx
+++ b/src/main/java/com/Dashboard/TestData/LoginTestData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaheen Akhtar\git\repository\Dashboard\src\main\java\com\Dashboard\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB1D9C4-4DDC-4E6E-9DCC-E3F5CFBED5ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12254DA-CD58-4789-BA15-DAE923C12B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2520" yWindow="1590" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{5957173E-284D-47B6-A290-4C6493186F86}"/>
   </bookViews>
@@ -507,7 +507,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,13 +530,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="C2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Send Email Module
</commit_message>
<xml_diff>
--- a/src/main/java/com/Dashboard/TestData/LoginTestData.xlsx
+++ b/src/main/java/com/Dashboard/TestData/LoginTestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaheen Akhtar\git\repository\Dashboard\src\main\java\com\Dashboard\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A12254DA-CD58-4789-BA15-DAE923C12B4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B44DE6A-9722-466C-87B9-592060A0C6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2520" yWindow="1590" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{5957173E-284D-47B6-A290-4C6493186F86}"/>
+    <workbookView xWindow="3405" yWindow="2565" windowWidth="15375" windowHeight="8040" activeTab="3" xr2:uid="{03447BB6-7A55-4885-90AE-844BDD6BE7C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="AddAlbum" sheetId="2" r:id="rId2"/>
     <sheet name="ChangePassword" sheetId="3" r:id="rId3"/>
+    <sheet name="SendEmail" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Email</t>
   </si>
@@ -48,31 +49,55 @@
     <t>dashboard@aimbeyond.com</t>
   </si>
   <si>
+    <t>test123</t>
+  </si>
+  <si>
     <t>Add_Album</t>
   </si>
   <si>
     <t>Description</t>
   </si>
   <si>
+    <t>Fest2</t>
+  </si>
+  <si>
     <t>test</t>
   </si>
   <si>
-    <t>Fest2</t>
+    <t>Old Password</t>
   </si>
   <si>
     <t>New Password</t>
   </si>
   <si>
-    <t>Old Password</t>
-  </si>
-  <si>
     <t>Confirm Password</t>
   </si>
   <si>
-    <t>test123</t>
-  </si>
-  <si>
     <t>test1234</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Bcc</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Body</t>
+  </si>
+  <si>
+    <t>shaheen.akhtar@aimbeyond.com</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>This is a test email.</t>
   </si>
 </sst>
 </file>
@@ -434,11 +459,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12940D30-8AEB-4E2D-8C72-6A29927993D2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73E19B13-A491-42BA-A382-21727D9F073A}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -459,34 +484,34 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{286819FC-4A75-49C2-98B3-CF110C957342}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A5CB97-CDDD-47B7-82BF-FB1B25E8131E}">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -494,7 +519,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -503,11 +528,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A31C90-BF1A-46C7-859A-74A941160E3F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF8CB3F7-F13C-4168-BDA4-834FD5563835}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -522,10 +547,10 @@
         <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -533,14 +558,73 @@
         <v>11</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD137960-DB55-4058-9407-7038EE66D0E3}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="A3:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{2802BE23-FDE2-4210-8772-AE6A9615A118}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{B09A2D5A-F22F-49A1-BA6C-0AAA1EE9A08B}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{3DFCEE18-DC24-4F87-B477-ED681E775B9A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added View Monthly Attendance module
</commit_message>
<xml_diff>
--- a/src/main/java/com/Dashboard/TestData/LoginTestData.xlsx
+++ b/src/main/java/com/Dashboard/TestData/LoginTestData.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaheen Akhtar\git\repository\Dashboard\src\main\java\com\Dashboard\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B44DE6A-9722-466C-87B9-592060A0C6D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE4CDBC-EB49-4CAB-A472-6E12509676E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="2565" windowWidth="15375" windowHeight="8040" activeTab="3" xr2:uid="{03447BB6-7A55-4885-90AE-844BDD6BE7C1}"/>
+    <workbookView xWindow="3405" yWindow="2565" windowWidth="15375" windowHeight="8040" firstSheet="2" activeTab="4" xr2:uid="{03447BB6-7A55-4885-90AE-844BDD6BE7C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
     <sheet name="AddAlbum" sheetId="2" r:id="rId2"/>
     <sheet name="ChangePassword" sheetId="3" r:id="rId3"/>
     <sheet name="SendEmail" sheetId="4" r:id="rId4"/>
+    <sheet name="ViewMonthlyAttendance" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Email</t>
   </si>
@@ -98,13 +99,28 @@
   </si>
   <si>
     <t>This is a test email.</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Month</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2018 </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +132,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -138,15 +161,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -463,7 +492,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD137960-DB55-4058-9407-7038EE66D0E3}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E3" sqref="A3:E3"/>
     </sheetView>
   </sheetViews>
@@ -627,4 +656,36 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C626CF-359B-439F-8DB6-D91F1FF3BFC2}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="A3:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Configuration issue resolved and all the tests are working as expected
</commit_message>
<xml_diff>
--- a/src/main/java/com/Dashboard/TestData/LoginTestData.xlsx
+++ b/src/main/java/com/Dashboard/TestData/LoginTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shaheen Akhtar\git\repository\Dashboard\src\main\java\com\Dashboard\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DE4CDBC-EB49-4CAB-A472-6E12509676E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{429EE9F6-98A6-49E8-BEE1-6C9A2137744C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="2565" windowWidth="15375" windowHeight="8040" firstSheet="2" activeTab="4" xr2:uid="{03447BB6-7A55-4885-90AE-844BDD6BE7C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="4" xr2:uid="{03447BB6-7A55-4885-90AE-844BDD6BE7C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -59,9 +59,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>Fest2</t>
-  </si>
-  <si>
     <t>test</t>
   </si>
   <si>
@@ -111,6 +108,9 @@
   </si>
   <si>
     <t xml:space="preserve">2018 </t>
+  </si>
+  <si>
+    <t>FestT</t>
   </si>
 </sst>
 </file>
@@ -526,7 +526,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,10 +545,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -573,18 +573,18 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>3</v>
@@ -616,36 +616,36 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
-      </c>
-      <c r="E1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -670,18 +670,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>